<commit_message>
Metrics from GitHub. Also used to assess individual contribution.
</commit_message>
<xml_diff>
--- a/Documentation/Contribution spreadsheet.xlsx
+++ b/Documentation/Contribution spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Devops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CEBE31-FCC4-4BD0-842D-6A82357E9980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED34C80-7433-4131-BEB7-3E322CB9101F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BB851CD8-CD76-4DA8-BF79-EB935EF2FE0F}"/>
   </bookViews>
@@ -84,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +101,13 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -130,11 +137,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -146,10 +154,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FE961530-2442-47A7-BB67-B0C1EE71848F}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -464,7 +474,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,14 +553,30 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="B3" s="6">
+        <v>45324</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">

</xml_diff>